<commit_message>
commit to checkout other branch
</commit_message>
<xml_diff>
--- a/data/Anmeldung_Landesmeisterschaft_2025.xlsx
+++ b/data/Anmeldung_Landesmeisterschaft_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leoni2/PycharmProjects/unicycle_score_board/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9CAB4A4-9271-CC40-884C-86F6B0182ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886013FA-B2EC-2B4A-B464-4B449CD8A876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27300" windowHeight="14200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="92">
   <si>
     <t>Freestyle Landesmeisterschaft von SH &amp; HH</t>
   </si>
@@ -546,6 +546,9 @@
   </si>
   <si>
     <t>Gravity Shift</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -2041,264 +2044,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -2323,6 +2068,264 @@
     <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2708,10 +2711,10 @@
       <c r="A4" s="112"/>
       <c r="B4" s="112"/>
       <c r="C4" s="112"/>
-      <c r="D4" s="182" t="s">
+      <c r="D4" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="182"/>
+      <c r="E4" s="189"/>
       <c r="F4" s="112"/>
       <c r="G4" s="112"/>
       <c r="H4" s="112"/>
@@ -2733,10 +2736,10 @@
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="180" t="s">
+      <c r="D5" s="187" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="181"/>
+      <c r="E5" s="188"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -2855,8 +2858,8 @@
     <row r="10" spans="1:21" ht="16">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
-      <c r="C10" s="178"/>
-      <c r="D10" s="179"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="186"/>
       <c r="E10" s="107"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -4993,7 +4996,7 @@
   <dimension ref="A1:AD114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="80" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="26"/>
@@ -6158,25 +6161,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="35.25" customHeight="1">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="214" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
-      <c r="F1" s="184"/>
-      <c r="G1" s="184"/>
-      <c r="H1" s="184"/>
-      <c r="I1" s="184"/>
-      <c r="J1" s="184"/>
-      <c r="K1" s="184"/>
-      <c r="L1" s="184"/>
-      <c r="M1" s="184"/>
-      <c r="N1" s="184"/>
-      <c r="O1" s="184"/>
-      <c r="P1" s="184"/>
-      <c r="Q1" s="185"/>
+      <c r="B1" s="215"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="215"/>
+      <c r="G1" s="215"/>
+      <c r="H1" s="215"/>
+      <c r="I1" s="215"/>
+      <c r="J1" s="215"/>
+      <c r="K1" s="215"/>
+      <c r="L1" s="215"/>
+      <c r="M1" s="215"/>
+      <c r="N1" s="215"/>
+      <c r="O1" s="215"/>
+      <c r="P1" s="215"/>
+      <c r="Q1" s="216"/>
       <c r="R1" s="25"/>
       <c r="S1" s="25"/>
       <c r="T1" s="25"/>
@@ -6192,10 +6195,10 @@
       <c r="AD1" s="27"/>
     </row>
     <row r="2" spans="1:30" ht="20" customHeight="1">
-      <c r="A2" s="198"/>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
+      <c r="A2" s="229"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="230"/>
+      <c r="D2" s="230"/>
       <c r="E2" s="174"/>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
@@ -6224,34 +6227,34 @@
       <c r="AD2" s="29"/>
     </row>
     <row r="3" spans="1:30" ht="42" customHeight="1">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="231" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="201"/>
+      <c r="B3" s="232"/>
       <c r="C3" s="78" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="43"/>
-      <c r="E3" s="217" t="s">
+      <c r="E3" s="196" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="218"/>
-      <c r="G3" s="219"/>
-      <c r="H3" s="232" t="s">
+      <c r="F3" s="197"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="211" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="233"/>
-      <c r="J3" s="234"/>
-      <c r="K3" s="229" t="s">
+      <c r="I3" s="212"/>
+      <c r="J3" s="213"/>
+      <c r="K3" s="208" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="230"/>
-      <c r="M3" s="231"/>
-      <c r="N3" s="226" t="s">
+      <c r="L3" s="209"/>
+      <c r="M3" s="210"/>
+      <c r="N3" s="205" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="227"/>
-      <c r="P3" s="228"/>
+      <c r="O3" s="206"/>
+      <c r="P3" s="207"/>
       <c r="Q3" s="42"/>
       <c r="R3" s="30"/>
       <c r="S3" s="24"/>
@@ -6268,55 +6271,55 @@
       <c r="AD3" s="29"/>
     </row>
     <row r="4" spans="1:30" ht="26.25" customHeight="1">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="233" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="235" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="205" t="s">
+      <c r="D4" s="236" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="215" t="s">
+      <c r="E4" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="207" t="s">
+      <c r="F4" s="238" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="209" t="s">
+      <c r="G4" s="240" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="220" t="s">
+      <c r="H4" s="199" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="188" t="s">
+      <c r="I4" s="219" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="192" t="s">
+      <c r="J4" s="223" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="222" t="s">
+      <c r="K4" s="201" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="190" t="s">
+      <c r="L4" s="221" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="194" t="s">
+      <c r="M4" s="225" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="224" t="s">
+      <c r="N4" s="203" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="196" t="s">
+      <c r="O4" s="227" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="186" t="s">
+      <c r="P4" s="217" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="213" t="s">
+      <c r="Q4" s="192" t="s">
         <v>36</v>
       </c>
       <c r="R4" s="30"/>
@@ -6334,25 +6337,25 @@
       <c r="AD4" s="29"/>
     </row>
     <row r="5" spans="1:30" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A5" s="203"/>
-      <c r="B5" s="203"/>
+      <c r="A5" s="234"/>
+      <c r="B5" s="234"/>
       <c r="C5" s="10">
         <v>45779</v>
       </c>
-      <c r="D5" s="206"/>
-      <c r="E5" s="216"/>
-      <c r="F5" s="208"/>
-      <c r="G5" s="210"/>
-      <c r="H5" s="221"/>
-      <c r="I5" s="189"/>
-      <c r="J5" s="193"/>
-      <c r="K5" s="223"/>
-      <c r="L5" s="191"/>
-      <c r="M5" s="195"/>
-      <c r="N5" s="225"/>
-      <c r="O5" s="197"/>
-      <c r="P5" s="187"/>
-      <c r="Q5" s="214"/>
+      <c r="D5" s="237"/>
+      <c r="E5" s="195"/>
+      <c r="F5" s="239"/>
+      <c r="G5" s="241"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="220"/>
+      <c r="J5" s="224"/>
+      <c r="K5" s="202"/>
+      <c r="L5" s="222"/>
+      <c r="M5" s="226"/>
+      <c r="N5" s="204"/>
+      <c r="O5" s="228"/>
+      <c r="P5" s="218"/>
+      <c r="Q5" s="193"/>
       <c r="R5" s="30"/>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
@@ -6492,10 +6495,10 @@
       <c r="AD7" s="33"/>
     </row>
     <row r="8" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A8" s="259" t="s">
+      <c r="A8" s="179" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="258">
+      <c r="B8" s="178">
         <v>37460</v>
       </c>
       <c r="C8" s="57">
@@ -6511,7 +6514,7 @@
       <c r="F8" s="145" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="261" t="s">
+      <c r="G8" s="181" t="s">
         <v>44</v>
       </c>
       <c r="H8" s="149"/>
@@ -6546,10 +6549,10 @@
       <c r="AD8" s="29"/>
     </row>
     <row r="9" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A9" s="260" t="s">
+      <c r="A9" s="180" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="258">
+      <c r="B9" s="178">
         <v>38296</v>
       </c>
       <c r="C9" s="65">
@@ -6562,10 +6565,10 @@
       <c r="E9" s="144" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="261" t="s">
+      <c r="F9" s="181" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="261" t="s">
+      <c r="G9" s="181" t="s">
         <v>41</v>
       </c>
       <c r="H9" s="68"/>
@@ -6600,10 +6603,10 @@
       <c r="AD9" s="29"/>
     </row>
     <row r="10" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A10" s="260" t="s">
+      <c r="A10" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="258">
+      <c r="B10" s="178">
         <v>37695</v>
       </c>
       <c r="C10" s="65">
@@ -6619,10 +6622,10 @@
       <c r="H10" s="149" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="262" t="s">
+      <c r="I10" s="182" t="s">
         <v>85</v>
       </c>
-      <c r="J10" s="262" t="s">
+      <c r="J10" s="182" t="s">
         <v>44</v>
       </c>
       <c r="K10" s="70"/>
@@ -6654,10 +6657,10 @@
       <c r="AD10" s="29"/>
     </row>
     <row r="11" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="180" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="258">
+      <c r="B11" s="178">
         <v>37509</v>
       </c>
       <c r="C11" s="65">
@@ -6673,10 +6676,10 @@
       <c r="H11" s="149" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="262" t="s">
+      <c r="I11" s="182" t="s">
         <v>85</v>
       </c>
-      <c r="J11" s="262" t="s">
+      <c r="J11" s="182" t="s">
         <v>44</v>
       </c>
       <c r="K11" s="70"/>
@@ -6708,10 +6711,10 @@
       <c r="AD11" s="29"/>
     </row>
     <row r="12" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A12" s="260" t="s">
+      <c r="A12" s="180" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="258">
+      <c r="B12" s="178">
         <v>38504</v>
       </c>
       <c r="C12" s="65">
@@ -6730,10 +6733,10 @@
       <c r="K12" s="149" t="s">
         <v>42</v>
       </c>
-      <c r="L12" s="263" t="s">
+      <c r="L12" s="183" t="s">
         <v>90</v>
       </c>
-      <c r="M12" s="264" t="s">
+      <c r="M12" s="184" t="s">
         <v>47</v>
       </c>
       <c r="N12" s="149" t="s">
@@ -6762,10 +6765,10 @@
       <c r="AD12" s="29"/>
     </row>
     <row r="13" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A13" s="260" t="s">
+      <c r="A13" s="180" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="258">
+      <c r="B13" s="178">
         <v>38401</v>
       </c>
       <c r="C13" s="65">
@@ -6784,10 +6787,10 @@
       <c r="K13" s="149" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="263" t="s">
+      <c r="L13" s="183" t="s">
         <v>90</v>
       </c>
-      <c r="M13" s="264" t="s">
+      <c r="M13" s="184" t="s">
         <v>47</v>
       </c>
       <c r="N13" s="149" t="s">
@@ -6816,10 +6819,10 @@
       <c r="AD13" s="29"/>
     </row>
     <row r="14" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A14" s="260" t="s">
+      <c r="A14" s="180" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="258">
+      <c r="B14" s="178">
         <v>38330</v>
       </c>
       <c r="C14" s="65">
@@ -6838,10 +6841,10 @@
       <c r="K14" s="149" t="s">
         <v>42</v>
       </c>
-      <c r="L14" s="263" t="s">
+      <c r="L14" s="183" t="s">
         <v>90</v>
       </c>
-      <c r="M14" s="264" t="s">
+      <c r="M14" s="184" t="s">
         <v>47</v>
       </c>
       <c r="N14" s="72"/>
@@ -6866,10 +6869,10 @@
       <c r="AD14" s="29"/>
     </row>
     <row r="15" spans="1:30" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A15" s="260" t="s">
+      <c r="A15" s="180" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="258">
+      <c r="B15" s="178">
         <v>37921</v>
       </c>
       <c r="C15" s="65">
@@ -6888,10 +6891,10 @@
       <c r="K15" s="149" t="s">
         <v>42</v>
       </c>
-      <c r="L15" s="263" t="s">
+      <c r="L15" s="183" t="s">
         <v>90</v>
       </c>
-      <c r="M15" s="264" t="s">
+      <c r="M15" s="184" t="s">
         <v>47</v>
       </c>
       <c r="N15" s="72"/>
@@ -7018,7 +7021,9 @@
       <c r="R18" s="28"/>
       <c r="S18" s="23"/>
       <c r="T18" s="23"/>
-      <c r="U18" s="23"/>
+      <c r="U18" s="23" t="s">
+        <v>91</v>
+      </c>
       <c r="V18" s="23"/>
       <c r="W18" s="24"/>
       <c r="X18" s="24"/>
@@ -8450,10 +8455,10 @@
       <c r="L56" s="140"/>
       <c r="M56" s="140"/>
       <c r="N56" s="139"/>
-      <c r="O56" s="211" t="s">
+      <c r="O56" s="190" t="s">
         <v>50</v>
       </c>
-      <c r="P56" s="212"/>
+      <c r="P56" s="191"/>
       <c r="Q56" s="170">
         <f>SUM(Q8:Q55)</f>
         <v>92</v>
@@ -10318,16 +10323,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="O56:P56"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="I4:I5"/>
@@ -10342,6 +10337,16 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
+    <mergeCell ref="O56:P56"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Diese Spalte bitte nicht ausfüllen" prompt="Diese Spalte bitte nicht ausfüllen" sqref="C6:C55" xr:uid="{31B8AB7E-14F6-4C46-925A-C2EA34D6270C}">
@@ -10399,26 +10404,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" ht="33.5" customHeight="1">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="246" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
-      <c r="M1" s="240"/>
-      <c r="N1" s="240"/>
-      <c r="O1" s="240"/>
-      <c r="P1" s="240"/>
-      <c r="Q1" s="240"/>
-      <c r="R1" s="240"/>
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="247"/>
+      <c r="E1" s="247"/>
+      <c r="F1" s="247"/>
+      <c r="G1" s="247"/>
+      <c r="H1" s="247"/>
+      <c r="I1" s="247"/>
+      <c r="J1" s="247"/>
+      <c r="K1" s="247"/>
+      <c r="L1" s="247"/>
+      <c r="M1" s="247"/>
+      <c r="N1" s="247"/>
+      <c r="O1" s="247"/>
+      <c r="P1" s="247"/>
+      <c r="Q1" s="247"/>
+      <c r="R1" s="247"/>
       <c r="S1" s="11"/>
       <c r="T1" s="11"/>
       <c r="U1" s="11"/>
@@ -10489,26 +10494,26 @@
       <c r="AP2" s="11"/>
     </row>
     <row r="3" spans="1:42" ht="52.5" customHeight="1">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="248" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="242"/>
-      <c r="C3" s="242"/>
-      <c r="D3" s="242"/>
-      <c r="E3" s="242"/>
-      <c r="F3" s="242"/>
-      <c r="G3" s="242"/>
-      <c r="H3" s="242"/>
-      <c r="I3" s="242"/>
-      <c r="J3" s="242"/>
-      <c r="K3" s="242"/>
-      <c r="L3" s="242"/>
-      <c r="M3" s="242"/>
-      <c r="N3" s="242"/>
-      <c r="O3" s="242"/>
-      <c r="P3" s="242"/>
-      <c r="Q3" s="242"/>
-      <c r="R3" s="242"/>
+      <c r="B3" s="249"/>
+      <c r="C3" s="249"/>
+      <c r="D3" s="249"/>
+      <c r="E3" s="249"/>
+      <c r="F3" s="249"/>
+      <c r="G3" s="249"/>
+      <c r="H3" s="249"/>
+      <c r="I3" s="249"/>
+      <c r="J3" s="249"/>
+      <c r="K3" s="249"/>
+      <c r="L3" s="249"/>
+      <c r="M3" s="249"/>
+      <c r="N3" s="249"/>
+      <c r="O3" s="249"/>
+      <c r="P3" s="249"/>
+      <c r="Q3" s="249"/>
+      <c r="R3" s="249"/>
       <c r="S3" s="123"/>
       <c r="T3" s="121"/>
       <c r="U3" s="121"/>
@@ -10516,20 +10521,20 @@
       <c r="W3" s="11"/>
       <c r="X3" s="11"/>
       <c r="Y3" s="11"/>
-      <c r="Z3" s="238"/>
-      <c r="AA3" s="238"/>
-      <c r="AB3" s="238"/>
-      <c r="AC3" s="238"/>
-      <c r="AD3" s="238"/>
-      <c r="AE3" s="238"/>
-      <c r="AF3" s="238"/>
-      <c r="AG3" s="238"/>
-      <c r="AH3" s="238"/>
-      <c r="AI3" s="238"/>
-      <c r="AJ3" s="238"/>
-      <c r="AK3" s="238"/>
-      <c r="AL3" s="238"/>
-      <c r="AM3" s="238"/>
+      <c r="Z3" s="245"/>
+      <c r="AA3" s="245"/>
+      <c r="AB3" s="245"/>
+      <c r="AC3" s="245"/>
+      <c r="AD3" s="245"/>
+      <c r="AE3" s="245"/>
+      <c r="AF3" s="245"/>
+      <c r="AG3" s="245"/>
+      <c r="AH3" s="245"/>
+      <c r="AI3" s="245"/>
+      <c r="AJ3" s="245"/>
+      <c r="AK3" s="245"/>
+      <c r="AL3" s="245"/>
+      <c r="AM3" s="245"/>
       <c r="AN3" s="11"/>
       <c r="AO3" s="11"/>
       <c r="AP3" s="11"/>
@@ -10539,26 +10544,26 @@
       <c r="B4" s="165"/>
       <c r="C4" s="166"/>
       <c r="D4" s="166"/>
-      <c r="E4" s="249" t="s">
+      <c r="E4" s="256" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="249"/>
-      <c r="G4" s="250" t="s">
+      <c r="F4" s="256"/>
+      <c r="G4" s="257" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="252" t="s">
+      <c r="H4" s="258"/>
+      <c r="I4" s="258"/>
+      <c r="J4" s="258"/>
+      <c r="K4" s="259" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="249"/>
-      <c r="M4" s="249"/>
-      <c r="N4" s="249"/>
-      <c r="O4" s="249"/>
-      <c r="P4" s="249"/>
-      <c r="Q4" s="249"/>
-      <c r="R4" s="253"/>
+      <c r="L4" s="256"/>
+      <c r="M4" s="256"/>
+      <c r="N4" s="256"/>
+      <c r="O4" s="256"/>
+      <c r="P4" s="256"/>
+      <c r="Q4" s="256"/>
+      <c r="R4" s="260"/>
       <c r="S4" s="123"/>
       <c r="T4" s="121"/>
       <c r="U4" s="121"/>
@@ -10585,16 +10590,16 @@
       <c r="AP4" s="11"/>
     </row>
     <row r="5" spans="1:42" ht="16">
-      <c r="A5" s="243" t="s">
+      <c r="A5" s="250" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="245" t="s">
+      <c r="B5" s="252" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="245" t="s">
+      <c r="D5" s="252" t="s">
         <v>56</v>
       </c>
       <c r="E5" s="176" t="s">
@@ -10615,22 +10620,22 @@
       <c r="J5" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="246" t="s">
+      <c r="K5" s="253" t="s">
         <v>58</v>
       </c>
-      <c r="L5" s="247"/>
-      <c r="M5" s="248" t="s">
+      <c r="L5" s="254"/>
+      <c r="M5" s="255" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="248"/>
-      <c r="O5" s="235" t="s">
+      <c r="N5" s="255"/>
+      <c r="O5" s="242" t="s">
         <v>60</v>
       </c>
-      <c r="P5" s="235"/>
-      <c r="Q5" s="236" t="s">
+      <c r="P5" s="242"/>
+      <c r="Q5" s="243" t="s">
         <v>61</v>
       </c>
-      <c r="R5" s="237"/>
+      <c r="R5" s="244"/>
       <c r="S5" s="122"/>
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
@@ -10657,12 +10662,12 @@
       <c r="AP5" s="11"/>
     </row>
     <row r="6" spans="1:42" ht="17" thickBot="1">
-      <c r="A6" s="244"/>
-      <c r="B6" s="244"/>
+      <c r="A6" s="251"/>
+      <c r="B6" s="251"/>
       <c r="C6" s="53">
         <v>45779</v>
       </c>
-      <c r="D6" s="244"/>
+      <c r="D6" s="251"/>
       <c r="E6" s="80" t="s">
         <v>62</v>
       </c>
@@ -11353,12 +11358,12 @@
     <row r="4" spans="1:22" ht="31">
       <c r="A4" s="111"/>
       <c r="B4" s="112"/>
-      <c r="C4" s="256" t="s">
+      <c r="C4" s="263" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="182"/>
-      <c r="E4" s="182"/>
-      <c r="F4" s="257"/>
+      <c r="D4" s="189"/>
+      <c r="E4" s="189"/>
+      <c r="F4" s="264"/>
       <c r="G4" s="112"/>
       <c r="H4" s="112"/>
       <c r="I4" s="11"/>
@@ -11380,10 +11385,10 @@
       <c r="A5" s="117"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="181" t="s">
+      <c r="D5" s="188" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="181"/>
+      <c r="E5" s="188"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -11410,10 +11415,10 @@
       <c r="A7" s="21"/>
       <c r="B7" s="103"/>
       <c r="C7" s="21"/>
-      <c r="D7" s="254" t="s">
+      <c r="D7" s="261" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="255"/>
+      <c r="E7" s="262"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>

</xml_diff>